<commit_message>
router revised and refined
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="40">
   <si>
     <t>index</t>
   </si>
@@ -105,9 +105,6 @@
     <t>leva ao overview</t>
   </si>
   <si>
-    <t>erro</t>
-  </si>
-  <si>
     <t>notas:</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>recover</t>
+  </si>
+  <si>
+    <t>desistir</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,12 +191,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -223,7 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,7 +516,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O17" sqref="O17"/>
+      <selection pane="topRight" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -583,10 +577,10 @@
       <c r="R1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="U1" t="s">
@@ -641,10 +635,16 @@
       <c r="P2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
+      <c r="Q2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
+      <c r="T2" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1" t="s">
         <v>25</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -675,7 +675,7 @@
         <v>25</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>25</v>
@@ -684,7 +684,7 @@
         <v>25</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>25</v>
@@ -694,8 +694,8 @@
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="2" t="s">
-        <v>24</v>
+      <c r="R3" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>24</v>
@@ -704,16 +704,16 @@
         <v>28</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="V3" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="V3" s="7"/>
       <c r="W3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -733,7 +733,7 @@
         <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>25</v>
@@ -742,7 +742,7 @@
         <v>25</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>25</v>
@@ -750,10 +750,14 @@
       <c r="O4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="R4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="3"/>
       <c r="U4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="V4" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="V4" s="7"/>
       <c r="W4" s="1" t="s">
         <v>25</v>
       </c>
@@ -764,7 +768,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>25</v>
@@ -779,25 +783,31 @@
         <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="M5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>36</v>
+      <c r="R5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>25</v>
@@ -825,13 +835,9 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="R6" s="1"/>
       <c r="S6" s="3"/>
-      <c r="T6" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="T6" s="1"/>
       <c r="U6" s="3"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -858,7 +864,7 @@
         <v>25</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>25</v>
@@ -867,7 +873,7 @@
         <v>25</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>25</v>
@@ -876,6 +882,8 @@
         <v>25</v>
       </c>
       <c r="P7" s="3"/>
+      <c r="R7" s="1"/>
+      <c r="T7" s="1"/>
       <c r="V7" s="1" t="s">
         <v>25</v>
       </c>
@@ -885,51 +893,55 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
       <c r="V8" s="5"/>
-      <c r="W8" s="8"/>
+      <c r="W8" s="7"/>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
+      <c r="S9" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="W12" s="1"/>
     </row>
     <row r="13" spans="1:23">
+      <c r="P13" s="8"/>
       <c r="W13" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
routes revised; universal filtering methods made, 2
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="41">
   <si>
     <t>index</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>desistir</t>
+  </si>
+  <si>
+    <t>filtros</t>
   </si>
 </sst>
 </file>
@@ -158,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +198,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -208,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -218,6 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,11 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q3" sqref="Q3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -535,7 +545,7 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F1" t="s">
@@ -568,10 +578,10 @@
       <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="9" t="s">
         <v>17</v>
       </c>
       <c r="R1" t="s">
@@ -586,7 +596,7 @@
       <c r="U1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="W1" t="s">
@@ -943,6 +953,13 @@
     <row r="13" spans="1:23">
       <c r="P13" s="8"/>
       <c r="W13" s="1"/>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="H14" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add to stock has issues
</commit_message>
<xml_diff>
--- a/routes.xlsx
+++ b/routes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="50">
   <si>
     <t>index</t>
   </si>
@@ -114,9 +114,6 @@
     <t>form (edit) | edit</t>
   </si>
   <si>
-    <t>ajustar</t>
-  </si>
-  <si>
     <t>remover link</t>
   </si>
   <si>
@@ -139,6 +136,36 @@
   </si>
   <si>
     <t>filtros</t>
+  </si>
+  <si>
+    <t>reativar</t>
+  </si>
+  <si>
+    <t>permissions!</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>permissions</t>
+  </si>
+  <si>
+    <t>n existem roles</t>
+  </si>
+  <si>
+    <t>sort n funciona</t>
+  </si>
+  <si>
+    <t>faltam os date-filters</t>
+  </si>
+  <si>
+    <t>o q fazer?</t>
+  </si>
+  <si>
+    <t>faltam os filtros</t>
+  </si>
+  <si>
+    <t>chamar a partir de orders</t>
   </si>
 </sst>
 </file>
@@ -155,7 +182,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,7 +226,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,11 +248,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -522,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H14" sqref="H14"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -535,7 +561,7 @@
     <col min="17" max="17" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -545,13 +571,13 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H1" t="s">
@@ -578,10 +604,10 @@
       <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="R1" t="s">
@@ -593,7 +619,7 @@
       <c r="T1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="V1" s="3" t="s">
@@ -602,19 +628,29 @@
       <c r="W1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
+      <c r="X1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>25</v>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
@@ -645,7 +681,7 @@
       <c r="P2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="R2" s="1" t="s">
@@ -663,18 +699,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
@@ -685,7 +725,7 @@
         <v>25</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>25</v>
@@ -694,7 +734,7 @@
         <v>25</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>25</v>
@@ -702,10 +742,12 @@
       <c r="O3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="3"/>
+      <c r="P3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="6"/>
       <c r="R3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>24</v>
@@ -714,25 +756,29 @@
         <v>28</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V3" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="V3" s="6"/>
       <c r="W3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
@@ -743,7 +789,7 @@
         <v>25</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>25</v>
@@ -752,7 +798,7 @@
         <v>25</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>25</v>
@@ -760,29 +806,36 @@
       <c r="O4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="P4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="6"/>
       <c r="R4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T4" s="3"/>
       <c r="U4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="V4" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="V4" s="6"/>
       <c r="W4" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
@@ -793,23 +846,27 @@
         <v>25</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="M5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="P5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q5" s="1"/>
       <c r="R5" s="1" t="s">
         <v>25</v>
       </c>
@@ -817,7 +874,7 @@
         <v>25</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>25</v>
@@ -826,14 +883,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -844,7 +901,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="3"/>
+      <c r="Q6" s="2"/>
       <c r="R6" s="1"/>
       <c r="S6" s="3"/>
       <c r="T6" s="1"/>
@@ -852,18 +909,22 @@
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>25</v>
       </c>
@@ -874,7 +935,7 @@
         <v>25</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>25</v>
@@ -883,7 +944,7 @@
         <v>25</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>25</v>
@@ -891,7 +952,9 @@
       <c r="O7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="R7" s="1"/>
       <c r="T7" s="1"/>
       <c r="V7" s="1" t="s">
@@ -901,65 +964,107 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="7"/>
-    </row>
-    <row r="9" spans="1:23">
+        <v>37</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
       <c r="S9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="W12" s="1"/>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="P13" s="7"/>
+      <c r="W13" s="1"/>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="W12" s="1"/>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="P13" s="8"/>
-      <c r="W13" s="1"/>
-    </row>
-    <row r="14" spans="1:23">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="1"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25">
+      <c r="R15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" s="9" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>